<commit_message>
Revamped templates, student/admin dashboard styling, OTP login
</commit_message>
<xml_diff>
--- a/Attendance Test.xlsx
+++ b/Attendance Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\attendance_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6D038C-7745-4778-BCB9-52A91FBF5118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1BA174-F7C4-46A0-8BF7-E42E66C408C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4692" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="13" xr2:uid="{A7955748-8F8E-4629-9B7A-DC1BC8E73719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="6" activeTab="13" xr2:uid="{A7955748-8F8E-4629-9B7A-DC1BC8E73719}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1 2022" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="507">
   <si>
     <t>First Name</t>
   </si>
@@ -1568,6 +1568,9 @@
   <si>
     <t>Noordeep Singh</t>
   </si>
+  <si>
+    <t xml:space="preserve">Kirtan </t>
+  </si>
 </sst>
 </file>
 
@@ -1716,7 +1719,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1924,6 +1927,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1931,7 +1945,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2075,6 +2089,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10049,10 +10070,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98E0ED3-A009-44A3-BB55-5421E7309795}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:M184"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="D181" sqref="D181:L181"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17599,8 +17620,43 @@
         <v>0.35262808641975307</v>
       </c>
     </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A185" s="63">
+        <v>20241077</v>
+      </c>
+      <c r="B185" s="63" t="s">
+        <v>506</v>
+      </c>
+      <c r="C185" s="63" t="s">
+        <v>422</v>
+      </c>
+      <c r="F185" s="64">
+        <v>1</v>
+      </c>
+      <c r="G185" s="64">
+        <v>1</v>
+      </c>
+      <c r="H185" s="64">
+        <v>1</v>
+      </c>
+      <c r="I185" s="64">
+        <v>1</v>
+      </c>
+      <c r="J185" s="64">
+        <v>1</v>
+      </c>
+      <c r="K185" s="64">
+        <v>1</v>
+      </c>
+      <c r="L185" s="64">
+        <v>1</v>
+      </c>
+      <c r="M185" s="65">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M2:M184">
+  <conditionalFormatting sqref="M2:M185">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.9</formula>
     </cfRule>
@@ -33988,8 +34044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA3181-CD29-4C7C-BAFB-910963920095}">
   <dimension ref="A1:L229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34060,8 +34116,8 @@
       <c r="I2" s="12">
         <v>0.86</v>
       </c>
-      <c r="J2" s="12">
-        <v>0.25</v>
+      <c r="J2" s="11">
+        <v>1.1299999999999999</v>
       </c>
       <c r="K2" s="12">
         <v>0.82</v>
@@ -34136,8 +34192,8 @@
       <c r="I4" s="11">
         <v>1.1399999999999999</v>
       </c>
-      <c r="J4" s="12">
-        <v>0.4</v>
+      <c r="J4" s="11">
+        <v>1.31</v>
       </c>
       <c r="K4" s="11">
         <v>1.2</v>
@@ -34175,7 +34231,7 @@
         <v>1.02</v>
       </c>
       <c r="J5" s="12">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="K5" s="11">
         <v>1.08</v>
@@ -34212,8 +34268,8 @@
       <c r="I6" s="11">
         <v>1.04</v>
       </c>
-      <c r="J6" s="12">
-        <v>0.33</v>
+      <c r="J6" s="11">
+        <v>1.23</v>
       </c>
       <c r="K6" s="11">
         <v>1.02</v>
@@ -34251,7 +34307,7 @@
         <v>0.78</v>
       </c>
       <c r="J7" s="12">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="K7" s="12">
         <v>0.74</v>
@@ -34289,7 +34345,7 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="12">
-        <v>0.22</v>
+        <v>0.53</v>
       </c>
       <c r="K8" s="12">
         <v>0</v>
@@ -34326,8 +34382,8 @@
       <c r="I9" s="11">
         <v>0.92</v>
       </c>
-      <c r="J9" s="12">
-        <v>0.3</v>
+      <c r="J9" s="11">
+        <v>1.22</v>
       </c>
       <c r="K9" s="11">
         <v>0.98</v>
@@ -34364,8 +34420,8 @@
       <c r="I10" s="12">
         <v>0.82</v>
       </c>
-      <c r="J10" s="12">
-        <v>0.31</v>
+      <c r="J10" s="11">
+        <v>1.23</v>
       </c>
       <c r="K10" s="11">
         <v>0.97</v>
@@ -34403,7 +34459,7 @@
         <v>0.78</v>
       </c>
       <c r="J11" s="12">
-        <v>0.4</v>
+        <v>0.86</v>
       </c>
       <c r="K11" s="11">
         <v>0.93</v>
@@ -34440,8 +34496,8 @@
       <c r="I12" s="11">
         <v>0.99</v>
       </c>
-      <c r="J12" s="12">
-        <v>0.74</v>
+      <c r="J12" s="11">
+        <v>1.31</v>
       </c>
       <c r="K12" s="11">
         <v>1.03</v>
@@ -34517,7 +34573,7 @@
         <v>0.85</v>
       </c>
       <c r="J14" s="12">
-        <v>0.32</v>
+        <v>0.86</v>
       </c>
       <c r="K14" s="12">
         <v>0.76</v>
@@ -34554,8 +34610,8 @@
       <c r="I15" s="12">
         <v>0.64</v>
       </c>
-      <c r="J15" s="12">
-        <v>0.37</v>
+      <c r="J15" s="11">
+        <v>1.23</v>
       </c>
       <c r="K15" s="11">
         <v>0.98</v>
@@ -34592,8 +34648,8 @@
       <c r="I16" s="12">
         <v>0.78</v>
       </c>
-      <c r="J16" s="12">
-        <v>0.41</v>
+      <c r="J16" s="11">
+        <v>1.04</v>
       </c>
       <c r="K16" s="12">
         <v>0.82</v>
@@ -34631,7 +34687,7 @@
         <v>0.43</v>
       </c>
       <c r="J17" s="12">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="K17" s="11">
         <v>1.24</v>
@@ -34668,8 +34724,8 @@
       <c r="I18" s="11">
         <v>0.99</v>
       </c>
-      <c r="J18" s="12">
-        <v>0.63</v>
+      <c r="J18" s="11">
+        <v>1.25</v>
       </c>
       <c r="K18" s="11">
         <v>1.02</v>
@@ -34706,8 +34762,8 @@
       <c r="I19" s="11">
         <v>1.07</v>
       </c>
-      <c r="J19" s="12">
-        <v>0.43</v>
+      <c r="J19" s="11">
+        <v>1.46</v>
       </c>
       <c r="K19" s="11">
         <v>1.05</v>
@@ -34733,22 +34789,22 @@
         <v>0.7</v>
       </c>
       <c r="F20" s="12">
-        <v>0.45</v>
+        <v>0.83</v>
       </c>
       <c r="G20" s="12">
         <v>0</v>
       </c>
       <c r="H20" s="12">
-        <v>0.26</v>
+        <v>0.76</v>
       </c>
       <c r="I20" s="12">
         <v>0.51</v>
       </c>
       <c r="J20" s="12">
-        <v>0.26</v>
+        <v>0.67</v>
       </c>
       <c r="K20" s="12">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="L20" s="11">
         <v>1</v>
@@ -34821,7 +34877,7 @@
         <v>0.99</v>
       </c>
       <c r="J22" s="12">
-        <v>0.38</v>
+        <v>0.87</v>
       </c>
       <c r="K22" s="11">
         <v>1.04</v>
@@ -34859,7 +34915,7 @@
         <v>0.64</v>
       </c>
       <c r="J23" s="12">
-        <v>0.31</v>
+        <v>0.87</v>
       </c>
       <c r="K23" s="11">
         <v>1.02</v>
@@ -34935,7 +34991,7 @@
         <v>1.06</v>
       </c>
       <c r="J25" s="12">
-        <v>0.36</v>
+        <v>0.86</v>
       </c>
       <c r="K25" s="11">
         <v>1.01</v>
@@ -34958,7 +35014,7 @@
         <v>0.9</v>
       </c>
       <c r="E26" s="12">
-        <v>0.18</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F26" s="11">
         <v>0.99</v>
@@ -34973,7 +35029,7 @@
         <v>0.68</v>
       </c>
       <c r="J26" s="12">
-        <v>0.39</v>
+        <v>0.49</v>
       </c>
       <c r="K26" s="12">
         <v>0.67</v>
@@ -35010,8 +35066,8 @@
       <c r="I27" s="11">
         <v>1.02</v>
       </c>
-      <c r="J27" s="12">
-        <v>0.34</v>
+      <c r="J27" s="11">
+        <v>1.32</v>
       </c>
       <c r="K27" s="11">
         <v>1.1399999999999999</v>
@@ -35048,8 +35104,8 @@
       <c r="I28" s="11">
         <v>1.04</v>
       </c>
-      <c r="J28" s="12">
-        <v>0.31</v>
+      <c r="J28" s="11">
+        <v>1.26</v>
       </c>
       <c r="K28" s="11">
         <v>0.99</v>
@@ -35086,8 +35142,8 @@
       <c r="I29" s="11">
         <v>1</v>
       </c>
-      <c r="J29" s="12">
-        <v>0.52</v>
+      <c r="J29" s="11">
+        <v>1.29</v>
       </c>
       <c r="K29" s="11">
         <v>0.92</v>
@@ -35124,8 +35180,8 @@
       <c r="I30" s="12">
         <v>0.43</v>
       </c>
-      <c r="J30" s="12">
-        <v>0.4</v>
+      <c r="J30" s="11">
+        <v>1</v>
       </c>
       <c r="K30" s="11">
         <v>1.03</v>
@@ -35162,8 +35218,8 @@
       <c r="I31" s="11">
         <v>0.93</v>
       </c>
-      <c r="J31" s="12">
-        <v>0.48</v>
+      <c r="J31" s="11">
+        <v>1.17</v>
       </c>
       <c r="K31" s="12">
         <v>0.86</v>
@@ -35201,7 +35257,7 @@
         <v>0.24</v>
       </c>
       <c r="J32" s="12">
-        <v>0.36</v>
+        <v>0.45</v>
       </c>
       <c r="K32" s="12">
         <v>0.56999999999999995</v>
@@ -35238,8 +35294,8 @@
       <c r="I33" s="12">
         <v>0.8</v>
       </c>
-      <c r="J33" s="12">
-        <v>0.39</v>
+      <c r="J33" s="11">
+        <v>0.99</v>
       </c>
       <c r="K33" s="11">
         <v>1.01</v>
@@ -35276,8 +35332,8 @@
       <c r="I34" s="11">
         <v>1.01</v>
       </c>
-      <c r="J34" s="12">
-        <v>0.4</v>
+      <c r="J34" s="11">
+        <v>1.53</v>
       </c>
       <c r="K34" s="11">
         <v>0.97</v>
@@ -35352,8 +35408,8 @@
       <c r="I36" s="11">
         <v>0.94</v>
       </c>
-      <c r="J36" s="12">
-        <v>0.48</v>
+      <c r="J36" s="11">
+        <v>1.25</v>
       </c>
       <c r="K36" s="11">
         <v>0.99</v>
@@ -35390,8 +35446,8 @@
       <c r="I37" s="11">
         <v>1.08</v>
       </c>
-      <c r="J37" s="12">
-        <v>0.41</v>
+      <c r="J37" s="11">
+        <v>1.29</v>
       </c>
       <c r="K37" s="11">
         <v>1.03</v>
@@ -35429,7 +35485,7 @@
         <v>0.73</v>
       </c>
       <c r="J38" s="12">
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="K38" s="12">
         <v>0.72</v>
@@ -35466,8 +35522,8 @@
       <c r="I39" s="11">
         <v>0.98</v>
       </c>
-      <c r="J39" s="12">
-        <v>0.31</v>
+      <c r="J39" s="11">
+        <v>1.21</v>
       </c>
       <c r="K39" s="11">
         <v>0.98</v>
@@ -35542,8 +35598,8 @@
       <c r="I41" s="12">
         <v>0.51</v>
       </c>
-      <c r="J41" s="12">
-        <v>0.2</v>
+      <c r="J41" s="11">
+        <v>1.02</v>
       </c>
       <c r="K41" s="11">
         <v>1.06</v>
@@ -35580,11 +35636,11 @@
       <c r="I42" s="11">
         <v>0.96</v>
       </c>
-      <c r="J42" s="12">
-        <v>0.42</v>
-      </c>
-      <c r="K42" s="12">
-        <v>0.64</v>
+      <c r="J42" s="11">
+        <v>1.17</v>
+      </c>
+      <c r="K42" s="11">
+        <v>0.98</v>
       </c>
       <c r="L42" s="12">
         <v>0.68</v>
@@ -35618,8 +35674,8 @@
       <c r="I43" s="11">
         <v>0.94</v>
       </c>
-      <c r="J43" s="12">
-        <v>0</v>
+      <c r="J43" s="11">
+        <v>0.93</v>
       </c>
       <c r="K43" s="12">
         <v>0.74</v>
@@ -35657,7 +35713,7 @@
         <v>0.46</v>
       </c>
       <c r="J44" s="12">
-        <v>0.24</v>
+        <v>0.7</v>
       </c>
       <c r="K44" s="12">
         <v>0.56000000000000005</v>
@@ -35695,7 +35751,7 @@
         <v>0.73</v>
       </c>
       <c r="J45" s="12">
-        <v>0.24</v>
+        <v>0.75</v>
       </c>
       <c r="K45" s="12">
         <v>0.56000000000000005</v>
@@ -35733,7 +35789,7 @@
         <v>0.46</v>
       </c>
       <c r="J46" s="12">
-        <v>0.25</v>
+        <v>0.71</v>
       </c>
       <c r="K46" s="12">
         <v>0.56000000000000005</v>
@@ -35770,8 +35826,8 @@
       <c r="I47" s="11">
         <v>1.1200000000000001</v>
       </c>
-      <c r="J47" s="12">
-        <v>0.41</v>
+      <c r="J47" s="11">
+        <v>0.95</v>
       </c>
       <c r="K47" s="11">
         <v>1.0900000000000001</v>
@@ -35808,8 +35864,8 @@
       <c r="I48" s="12">
         <v>0.69</v>
       </c>
-      <c r="J48" s="12">
-        <v>0.45</v>
+      <c r="J48" s="11">
+        <v>1.07</v>
       </c>
       <c r="K48" s="12">
         <v>0.85</v>
@@ -35846,8 +35902,8 @@
       <c r="I49" s="12">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J49" s="12">
-        <v>0.56000000000000005</v>
+      <c r="J49" s="11">
+        <v>1.08</v>
       </c>
       <c r="K49" s="12">
         <v>0.73</v>
@@ -35884,8 +35940,8 @@
       <c r="I50" s="11">
         <v>0.99</v>
       </c>
-      <c r="J50" s="12">
-        <v>0.25</v>
+      <c r="J50" s="11">
+        <v>1.19</v>
       </c>
       <c r="K50" s="11">
         <v>0.97</v>
@@ -35923,7 +35979,7 @@
         <v>0.98</v>
       </c>
       <c r="J51" s="12">
-        <v>0.38</v>
+        <v>0.83</v>
       </c>
       <c r="K51" s="11">
         <v>0.96</v>
@@ -35961,7 +36017,7 @@
         <v>0.91</v>
       </c>
       <c r="J52" s="12">
-        <v>0.35</v>
+        <v>0.79</v>
       </c>
       <c r="K52" s="11">
         <v>0.95</v>
@@ -35999,7 +36055,7 @@
         <v>0.66</v>
       </c>
       <c r="J53" s="12">
-        <v>0.33</v>
+        <v>0.77</v>
       </c>
       <c r="K53" s="12">
         <v>0.85</v>
@@ -36036,8 +36092,8 @@
       <c r="I54" s="12">
         <v>0.71</v>
       </c>
-      <c r="J54" s="12">
-        <v>0.27</v>
+      <c r="J54" s="11">
+        <v>0.97</v>
       </c>
       <c r="K54" s="12">
         <v>0.76</v>
@@ -36075,7 +36131,7 @@
         <v>0.59</v>
       </c>
       <c r="J55" s="12">
-        <v>0.28999999999999998</v>
+        <v>0.84</v>
       </c>
       <c r="K55" s="12">
         <v>0.71</v>
@@ -36112,8 +36168,8 @@
       <c r="I56" s="11">
         <v>0.98</v>
       </c>
-      <c r="J56" s="12">
-        <v>0.24</v>
+      <c r="J56" s="11">
+        <v>0.91</v>
       </c>
       <c r="K56" s="12">
         <v>0.67</v>
@@ -36151,7 +36207,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="J57" s="12">
-        <v>0.44</v>
+        <v>0.9</v>
       </c>
       <c r="K57" s="11">
         <v>1.05</v>
@@ -36189,7 +36245,7 @@
         <v>0.97</v>
       </c>
       <c r="J58" s="12">
-        <v>0.2</v>
+        <v>0.74</v>
       </c>
       <c r="K58" s="11">
         <v>1.03</v>
@@ -36227,7 +36283,7 @@
         <v>0.92</v>
       </c>
       <c r="J59" s="12">
-        <v>0.05</v>
+        <v>0.79</v>
       </c>
       <c r="K59" s="11">
         <v>1</v>
@@ -36302,8 +36358,8 @@
       <c r="I61" s="11">
         <v>0.96</v>
       </c>
-      <c r="J61" s="12">
-        <v>0.23</v>
+      <c r="J61" s="11">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K61" s="12">
         <v>0.43</v>
@@ -36378,8 +36434,8 @@
       <c r="I63" s="11">
         <v>0.95</v>
       </c>
-      <c r="J63" s="12">
-        <v>0.41</v>
+      <c r="J63" s="11">
+        <v>1.05</v>
       </c>
       <c r="K63" s="11">
         <v>1.02</v>
@@ -36405,7 +36461,7 @@
         <v>0.79</v>
       </c>
       <c r="F64" s="12">
-        <v>0.86</v>
+        <v>0.81</v>
       </c>
       <c r="G64" s="12">
         <v>0.9</v>
@@ -36417,7 +36473,7 @@
         <v>0.78</v>
       </c>
       <c r="J64" s="12">
-        <v>0.67</v>
+        <v>0.84</v>
       </c>
       <c r="K64" s="12">
         <v>0.84</v>
@@ -36454,8 +36510,8 @@
       <c r="I65" s="12">
         <v>0.78</v>
       </c>
-      <c r="J65" s="12">
-        <v>0.41</v>
+      <c r="J65" s="11">
+        <v>0.9</v>
       </c>
       <c r="K65" s="11">
         <v>0.95</v>
@@ -36493,7 +36549,7 @@
         <v>0.78</v>
       </c>
       <c r="J66" s="12">
-        <v>0.25</v>
+        <v>0.77</v>
       </c>
       <c r="K66" s="11">
         <v>1.07</v>
@@ -36530,8 +36586,8 @@
       <c r="I67" s="11">
         <v>1.02</v>
       </c>
-      <c r="J67" s="12">
-        <v>0.35</v>
+      <c r="J67" s="11">
+        <v>0.99</v>
       </c>
       <c r="K67" s="11">
         <v>0.99</v>
@@ -36569,7 +36625,7 @@
         <v>0.68</v>
       </c>
       <c r="J68" s="12">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="K68" s="12">
         <v>0.88</v>
@@ -36607,7 +36663,7 @@
         <v>0.94</v>
       </c>
       <c r="J69" s="12">
-        <v>0.28999999999999998</v>
+        <v>0.89</v>
       </c>
       <c r="K69" s="11">
         <v>1.01</v>
@@ -36644,8 +36700,8 @@
       <c r="I70" s="12">
         <v>0.51</v>
       </c>
-      <c r="J70" s="12">
-        <v>0.26</v>
+      <c r="J70" s="11">
+        <v>1.01</v>
       </c>
       <c r="K70" s="12">
         <v>0.52</v>
@@ -36682,8 +36738,8 @@
       <c r="I71" s="11">
         <v>1.01</v>
       </c>
-      <c r="J71" s="12">
-        <v>0.51</v>
+      <c r="J71" s="11">
+        <v>0.94</v>
       </c>
       <c r="K71" s="11">
         <v>1.01</v>
@@ -36720,8 +36776,8 @@
       <c r="I72" s="11">
         <v>0.96</v>
       </c>
-      <c r="J72" s="12">
-        <v>0.72</v>
+      <c r="J72" s="11">
+        <v>1.25</v>
       </c>
       <c r="K72" s="11">
         <v>1</v>
@@ -36758,8 +36814,8 @@
       <c r="I73" s="11">
         <v>1.28</v>
       </c>
-      <c r="J73" s="12">
-        <v>0.38</v>
+      <c r="J73" s="11">
+        <v>1.26</v>
       </c>
       <c r="K73" s="11">
         <v>1</v>
@@ -36797,7 +36853,7 @@
         <v>0.47</v>
       </c>
       <c r="J74" s="12">
-        <v>0.19</v>
+        <v>0.83</v>
       </c>
       <c r="K74" s="12">
         <v>0.5</v>
@@ -36835,7 +36891,7 @@
         <v>0.44</v>
       </c>
       <c r="J75" s="12">
-        <v>0.24</v>
+        <v>0.7</v>
       </c>
       <c r="K75" s="12">
         <v>0.56000000000000005</v>
@@ -36872,8 +36928,8 @@
       <c r="I76" s="11">
         <v>1</v>
       </c>
-      <c r="J76" s="12">
-        <v>0.45</v>
+      <c r="J76" s="11">
+        <v>1.29</v>
       </c>
       <c r="K76" s="11">
         <v>1.17</v>
@@ -36911,7 +36967,7 @@
         <v>0.67</v>
       </c>
       <c r="J77" s="12">
-        <v>0.33</v>
+        <v>0.82</v>
       </c>
       <c r="K77" s="11">
         <v>1</v>
@@ -36937,7 +36993,7 @@
         <v>0.85</v>
       </c>
       <c r="F78" s="12">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="G78" s="12">
         <v>0.84</v>
@@ -36949,7 +37005,7 @@
         <v>0.88</v>
       </c>
       <c r="J78" s="12">
-        <v>0.34</v>
+        <v>0.68</v>
       </c>
       <c r="K78" s="12">
         <v>0.66</v>
@@ -36986,8 +37042,8 @@
       <c r="I79" s="11">
         <v>1</v>
       </c>
-      <c r="J79" s="12">
-        <v>0.39</v>
+      <c r="J79" s="11">
+        <v>1.31</v>
       </c>
       <c r="K79" s="11">
         <v>1.05</v>
@@ -37013,7 +37069,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="12">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="G80" s="12">
         <v>0.36</v>
@@ -37025,7 +37081,7 @@
         <v>0.94</v>
       </c>
       <c r="J80" s="12">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="K80" s="11">
         <v>1.1499999999999999</v>
@@ -37048,7 +37104,7 @@
         <v>0.73</v>
       </c>
       <c r="E81" s="12">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="F81" s="12">
         <v>0.68</v>
@@ -37063,7 +37119,7 @@
         <v>0.49</v>
       </c>
       <c r="J81" s="12">
-        <v>0.37</v>
+        <v>0.89</v>
       </c>
       <c r="K81" s="12">
         <v>0.78</v>
@@ -37089,7 +37145,7 @@
         <v>0.98</v>
       </c>
       <c r="F82" s="11">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="G82" s="11">
         <v>1</v>
@@ -37100,8 +37156,8 @@
       <c r="I82" s="11">
         <v>0.95</v>
       </c>
-      <c r="J82" s="12">
-        <v>0.51</v>
+      <c r="J82" s="11">
+        <v>1.27</v>
       </c>
       <c r="K82" s="12">
         <v>0.84</v>
@@ -37138,8 +37194,8 @@
       <c r="I83" s="11">
         <v>0.91</v>
       </c>
-      <c r="J83" s="12">
-        <v>0.32</v>
+      <c r="J83" s="11">
+        <v>1.08</v>
       </c>
       <c r="K83" s="12">
         <v>0.74</v>
@@ -37177,7 +37233,7 @@
         <v>0.78</v>
       </c>
       <c r="J84" s="12">
-        <v>0.27</v>
+        <v>0.69</v>
       </c>
       <c r="K84" s="12">
         <v>0.86</v>
@@ -37215,7 +37271,7 @@
         <v>1</v>
       </c>
       <c r="J85" s="12">
-        <v>0.24</v>
+        <v>0.78</v>
       </c>
       <c r="K85" s="11">
         <v>1.01</v>
@@ -37244,7 +37300,7 @@
         <v>1.39</v>
       </c>
       <c r="G86" s="11">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="H86" s="12">
         <v>0.75</v>
@@ -37252,8 +37308,8 @@
       <c r="I86" s="11">
         <v>0.96</v>
       </c>
-      <c r="J86" s="12">
-        <v>0.31</v>
+      <c r="J86" s="11">
+        <v>1.23</v>
       </c>
       <c r="K86" s="11">
         <v>0.94</v>
@@ -37291,7 +37347,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="J87" s="12">
-        <v>0.41</v>
+        <v>0.84</v>
       </c>
       <c r="K87" s="11">
         <v>1.03</v>
@@ -37329,7 +37385,7 @@
         <v>0.77</v>
       </c>
       <c r="J88" s="12">
-        <v>0.39</v>
+        <v>0.49</v>
       </c>
       <c r="K88" s="12">
         <v>0.53</v>
@@ -37366,8 +37422,8 @@
       <c r="I89" s="12">
         <v>0.64</v>
       </c>
-      <c r="J89" s="12">
-        <v>0.37</v>
+      <c r="J89" s="11">
+        <v>1.22</v>
       </c>
       <c r="K89" s="11">
         <v>0.98</v>
@@ -37404,8 +37460,8 @@
       <c r="I90" s="11">
         <v>0.94</v>
       </c>
-      <c r="J90" s="12">
-        <v>0.37</v>
+      <c r="J90" s="11">
+        <v>1.06</v>
       </c>
       <c r="K90" s="11">
         <v>0.97</v>
@@ -37442,8 +37498,8 @@
       <c r="I91" s="11">
         <v>0.95</v>
       </c>
-      <c r="J91" s="12">
-        <v>0</v>
+      <c r="J91" s="11">
+        <v>0.93</v>
       </c>
       <c r="K91" s="12">
         <v>0.77</v>
@@ -37480,8 +37536,8 @@
       <c r="I92" s="11">
         <v>1.05</v>
       </c>
-      <c r="J92" s="12">
-        <v>0.31</v>
+      <c r="J92" s="11">
+        <v>1.26</v>
       </c>
       <c r="K92" s="11">
         <v>1.03</v>
@@ -37518,8 +37574,8 @@
       <c r="I93" s="11">
         <v>1.1299999999999999</v>
       </c>
-      <c r="J93" s="12">
-        <v>0.56000000000000005</v>
+      <c r="J93" s="11">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K93" s="12">
         <v>0.69</v>
@@ -37556,8 +37612,8 @@
       <c r="I94" s="11">
         <v>1.03</v>
       </c>
-      <c r="J94" s="12">
-        <v>0.42</v>
+      <c r="J94" s="11">
+        <v>0.93</v>
       </c>
       <c r="K94" s="12">
         <v>0.72</v>
@@ -37595,7 +37651,7 @@
         <v>1.05</v>
       </c>
       <c r="J95" s="12">
-        <v>0.34</v>
+        <v>0.8</v>
       </c>
       <c r="K95" s="12">
         <v>0.74</v>
@@ -37633,7 +37689,7 @@
         <v>0.91</v>
       </c>
       <c r="J96" s="12">
-        <v>0.37</v>
+        <v>0.88</v>
       </c>
       <c r="K96" s="12">
         <v>0.49</v>
@@ -37662,7 +37718,7 @@
         <v>1.08</v>
       </c>
       <c r="G97" s="12">
-        <v>0.42</v>
+        <v>0.88</v>
       </c>
       <c r="H97" s="12">
         <v>0.81</v>
@@ -37670,8 +37726,8 @@
       <c r="I97" s="12">
         <v>0.86</v>
       </c>
-      <c r="J97" s="12">
-        <v>0.4</v>
+      <c r="J97" s="11">
+        <v>1.03</v>
       </c>
       <c r="K97" s="12">
         <v>0.59</v>
@@ -37708,8 +37764,8 @@
       <c r="I98" s="11">
         <v>1</v>
       </c>
-      <c r="J98" s="12">
-        <v>0.51</v>
+      <c r="J98" s="11">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K98" s="11">
         <v>0.96</v>
@@ -37746,8 +37802,8 @@
       <c r="I99" s="12">
         <v>0.9</v>
       </c>
-      <c r="J99" s="12">
-        <v>0.34</v>
+      <c r="J99" s="11">
+        <v>0.99</v>
       </c>
       <c r="K99" s="12">
         <v>0.85</v>
@@ -37785,7 +37841,7 @@
         <v>0.64</v>
       </c>
       <c r="J100" s="12">
-        <v>0.22</v>
+        <v>0.79</v>
       </c>
       <c r="K100" s="11">
         <v>0.98</v>
@@ -37823,7 +37879,7 @@
         <v>0.94</v>
       </c>
       <c r="J101" s="12">
-        <v>0.2</v>
+        <v>0.84</v>
       </c>
       <c r="K101" s="11">
         <v>0.97</v>
@@ -37861,7 +37917,7 @@
         <v>0.71</v>
       </c>
       <c r="J102" s="12">
-        <v>0.28999999999999998</v>
+        <v>0.37</v>
       </c>
       <c r="K102" s="11">
         <v>0.95</v>
@@ -37898,8 +37954,8 @@
       <c r="I103" s="11">
         <v>1.31</v>
       </c>
-      <c r="J103" s="12">
-        <v>0.42</v>
+      <c r="J103" s="11">
+        <v>0.97</v>
       </c>
       <c r="K103" s="12">
         <v>0.68</v>
@@ -37925,7 +37981,7 @@
         <v>0.32</v>
       </c>
       <c r="F104" s="12">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="G104" s="12">
         <v>0.51</v>
@@ -37937,7 +37993,7 @@
         <v>0.37</v>
       </c>
       <c r="J104" s="12">
-        <v>0.34</v>
+        <v>0.69</v>
       </c>
       <c r="K104" s="12">
         <v>0.32</v>
@@ -37974,8 +38030,8 @@
       <c r="I105" s="11">
         <v>0.94</v>
       </c>
-      <c r="J105" s="12">
-        <v>0.49</v>
+      <c r="J105" s="11">
+        <v>1.21</v>
       </c>
       <c r="K105" s="11">
         <v>1.01</v>
@@ -38013,7 +38069,7 @@
         <v>1.17</v>
       </c>
       <c r="J106" s="12">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="K106" s="11">
         <v>1.06</v>
@@ -38050,8 +38106,8 @@
       <c r="I107" s="11">
         <v>1</v>
       </c>
-      <c r="J107" s="12">
-        <v>0.45</v>
+      <c r="J107" s="11">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K107" s="12">
         <v>0.39</v>
@@ -38088,8 +38144,8 @@
       <c r="I108" s="11">
         <v>0.96</v>
       </c>
-      <c r="J108" s="12">
-        <v>0.38</v>
+      <c r="J108" s="11">
+        <v>1.2</v>
       </c>
       <c r="K108" s="12">
         <v>0.89</v>
@@ -38127,7 +38183,7 @@
         <v>0.49</v>
       </c>
       <c r="J109" s="12">
-        <v>0.18</v>
+        <v>0.23</v>
       </c>
       <c r="K109" s="12">
         <v>0.41</v>
@@ -38164,8 +38220,8 @@
       <c r="I110" s="11">
         <v>1.06</v>
       </c>
-      <c r="J110" s="12">
-        <v>0.42</v>
+      <c r="J110" s="11">
+        <v>0.92</v>
       </c>
       <c r="K110" s="11">
         <v>1.07</v>
@@ -38202,8 +38258,8 @@
       <c r="I111" s="12">
         <v>0.52</v>
       </c>
-      <c r="J111" s="12">
-        <v>0.5</v>
+      <c r="J111" s="11">
+        <v>1.1200000000000001</v>
       </c>
       <c r="K111" s="11">
         <v>1.03</v>
@@ -38240,8 +38296,8 @@
       <c r="I112" s="11">
         <v>1.04</v>
       </c>
-      <c r="J112" s="12">
-        <v>0.27</v>
+      <c r="J112" s="11">
+        <v>1.23</v>
       </c>
       <c r="K112" s="12">
         <v>0.45</v>
@@ -38279,7 +38335,7 @@
         <v>1.17</v>
       </c>
       <c r="J113" s="12">
-        <v>0.4</v>
+        <v>0.78</v>
       </c>
       <c r="K113" s="11">
         <v>1.01</v>
@@ -38354,8 +38410,8 @@
       <c r="I115" s="11">
         <v>1.1299999999999999</v>
       </c>
-      <c r="J115" s="12">
-        <v>0.42</v>
+      <c r="J115" s="11">
+        <v>1.47</v>
       </c>
       <c r="K115" s="11">
         <v>1.1599999999999999</v>
@@ -38392,8 +38448,8 @@
       <c r="I116" s="12">
         <v>0.4</v>
       </c>
-      <c r="J116" s="12">
-        <v>0.35</v>
+      <c r="J116" s="11">
+        <v>1.26</v>
       </c>
       <c r="K116" s="12">
         <v>0.7</v>
@@ -38431,7 +38487,7 @@
         <v>1.01</v>
       </c>
       <c r="J117" s="12">
-        <v>0.51</v>
+        <v>0.87</v>
       </c>
       <c r="K117" s="11">
         <v>1.01</v>
@@ -38469,7 +38525,7 @@
         <v>1.03</v>
       </c>
       <c r="J118" s="12">
-        <v>0.12</v>
+        <v>0.81</v>
       </c>
       <c r="K118" s="11">
         <v>1.01</v>
@@ -38507,7 +38563,7 @@
         <v>0.82</v>
       </c>
       <c r="J119" s="12">
-        <v>0.28000000000000003</v>
+        <v>0.35</v>
       </c>
       <c r="K119" s="11">
         <v>1.04</v>
@@ -38545,7 +38601,7 @@
         <v>1.03</v>
       </c>
       <c r="J120" s="12">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K120" s="11">
         <v>1.04</v>
@@ -38582,8 +38638,8 @@
       <c r="I121" s="11">
         <v>0.95</v>
       </c>
-      <c r="J121" s="12">
-        <v>0.27</v>
+      <c r="J121" s="11">
+        <v>1.29</v>
       </c>
       <c r="K121" s="12">
         <v>0.77</v>
@@ -38620,8 +38676,8 @@
       <c r="I122" s="11">
         <v>1.1599999999999999</v>
       </c>
-      <c r="J122" s="12">
-        <v>0.36</v>
+      <c r="J122" s="11">
+        <v>1.23</v>
       </c>
       <c r="K122" s="11">
         <v>1.27</v>
@@ -38659,7 +38715,7 @@
         <v>0.89</v>
       </c>
       <c r="J123" s="12">
-        <v>0.1</v>
+        <v>0.62</v>
       </c>
       <c r="K123" s="12">
         <v>0.89</v>
@@ -38688,7 +38744,7 @@
         <v>0.95</v>
       </c>
       <c r="G124" s="11">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="H124" s="11">
         <v>1.1599999999999999</v>
@@ -38697,7 +38753,7 @@
         <v>0.99</v>
       </c>
       <c r="J124" s="12">
-        <v>0.42</v>
+        <v>0.83</v>
       </c>
       <c r="K124" s="12">
         <v>0.82</v>
@@ -38734,8 +38790,8 @@
       <c r="I125" s="12">
         <v>0.78</v>
       </c>
-      <c r="J125" s="12">
-        <v>0</v>
+      <c r="J125" s="11">
+        <v>0.93</v>
       </c>
       <c r="K125" s="12">
         <v>0.75</v>
@@ -38772,8 +38828,8 @@
       <c r="I126" s="11">
         <v>0.99</v>
       </c>
-      <c r="J126" s="12">
-        <v>0.26</v>
+      <c r="J126" s="11">
+        <v>0.94</v>
       </c>
       <c r="K126" s="11">
         <v>0.92</v>
@@ -38810,8 +38866,8 @@
       <c r="I127" s="11">
         <v>0.95</v>
       </c>
-      <c r="J127" s="12">
-        <v>0.25</v>
+      <c r="J127" s="11">
+        <v>1.1599999999999999</v>
       </c>
       <c r="K127" s="11">
         <v>1.25</v>
@@ -38849,7 +38905,7 @@
         <v>0.21</v>
       </c>
       <c r="J128" s="12">
-        <v>0.1</v>
+        <v>0.46</v>
       </c>
       <c r="K128" s="12">
         <v>0.11</v>
@@ -38886,8 +38942,8 @@
       <c r="I129" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J129" s="12">
-        <v>0</v>
+      <c r="J129" s="11">
+        <v>0.97</v>
       </c>
       <c r="K129" s="11">
         <v>1.07</v>
@@ -38916,7 +38972,7 @@
         <v>1.07</v>
       </c>
       <c r="G130" s="11">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H130" s="11">
         <v>1.34</v>
@@ -38924,8 +38980,8 @@
       <c r="I130" s="11">
         <v>1.0900000000000001</v>
       </c>
-      <c r="J130" s="12">
-        <v>0.34</v>
+      <c r="J130" s="11">
+        <v>1.28</v>
       </c>
       <c r="K130" s="11">
         <v>1.02</v>
@@ -38963,7 +39019,7 @@
         <v>1.02</v>
       </c>
       <c r="J131" s="12">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="K131" s="12">
         <v>0.7</v>
@@ -39001,7 +39057,7 @@
         <v>1.08</v>
       </c>
       <c r="J132" s="12">
-        <v>0.32</v>
+        <v>0.74</v>
       </c>
       <c r="K132" s="11">
         <v>0.92</v>
@@ -39038,8 +39094,8 @@
       <c r="I133" s="11">
         <v>0.96</v>
       </c>
-      <c r="J133" s="12">
-        <v>0.56999999999999995</v>
+      <c r="J133" s="11">
+        <v>0.93</v>
       </c>
       <c r="K133" s="11">
         <v>1.22</v>
@@ -39076,8 +39132,8 @@
       <c r="I134" s="11">
         <v>1.25</v>
       </c>
-      <c r="J134" s="12">
-        <v>0</v>
+      <c r="J134" s="11">
+        <v>0.92</v>
       </c>
       <c r="K134" s="11">
         <v>1.1299999999999999</v>
@@ -39114,8 +39170,8 @@
       <c r="I135" s="12">
         <v>0.31</v>
       </c>
-      <c r="J135" s="12">
-        <v>0</v>
+      <c r="J135" s="11">
+        <v>0.93</v>
       </c>
       <c r="K135" s="12">
         <v>0.72</v>
@@ -39153,7 +39209,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="J136" s="12">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="K136" s="11">
         <v>1.17</v>
@@ -39191,7 +39247,7 @@
         <v>1.03</v>
       </c>
       <c r="J137" s="12">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="K137" s="11">
         <v>1.02</v>
@@ -39229,7 +39285,7 @@
         <v>0.52</v>
       </c>
       <c r="J138" s="12">
-        <v>0.31</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K138" s="12">
         <v>0.61</v>
@@ -39266,8 +39322,8 @@
       <c r="I139" s="11">
         <v>1.03</v>
       </c>
-      <c r="J139" s="12">
-        <v>0.33</v>
+      <c r="J139" s="11">
+        <v>1.28</v>
       </c>
       <c r="K139" s="11">
         <v>1.07</v>
@@ -39305,7 +39361,7 @@
         <v>0.8</v>
       </c>
       <c r="J140" s="12">
-        <v>0.2</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K140" s="12">
         <v>0.17</v>
@@ -39343,7 +39399,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="J141" s="12">
-        <v>0.17</v>
+        <v>0.26</v>
       </c>
       <c r="K141" s="11">
         <v>1</v>
@@ -39380,8 +39436,8 @@
       <c r="I142" s="11">
         <v>1.17</v>
       </c>
-      <c r="J142" s="12">
-        <v>0.36</v>
+      <c r="J142" s="11">
+        <v>1.31</v>
       </c>
       <c r="K142" s="11">
         <v>1.1100000000000001</v>
@@ -39419,7 +39475,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="J143" s="12">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="K143" s="12">
         <v>0.68</v>
@@ -39457,7 +39513,7 @@
         <v>0.93</v>
       </c>
       <c r="J144" s="12">
-        <v>0.33</v>
+        <v>0.42</v>
       </c>
       <c r="K144" s="11">
         <v>1.07</v>
@@ -39495,7 +39551,7 @@
         <v>0.97</v>
       </c>
       <c r="J145" s="12">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="K145" s="11">
         <v>1.02</v>
@@ -39532,8 +39588,8 @@
       <c r="I146" s="11">
         <v>1.03</v>
       </c>
-      <c r="J146" s="12">
-        <v>0</v>
+      <c r="J146" s="11">
+        <v>0.9</v>
       </c>
       <c r="K146" s="11">
         <v>1.01</v>
@@ -39570,8 +39626,8 @@
       <c r="I147" s="11">
         <v>0.97</v>
       </c>
-      <c r="J147" s="12">
-        <v>0.37</v>
+      <c r="J147" s="11">
+        <v>0.99</v>
       </c>
       <c r="K147" s="11">
         <v>1.07</v>
@@ -39608,8 +39664,8 @@
       <c r="I148" s="12">
         <v>0.89</v>
       </c>
-      <c r="J148" s="12">
-        <v>0.48</v>
+      <c r="J148" s="11">
+        <v>1.03</v>
       </c>
       <c r="K148" s="11">
         <v>1.02</v>
@@ -39646,8 +39702,8 @@
       <c r="I149" s="11">
         <v>1.21</v>
       </c>
-      <c r="J149" s="12">
-        <v>0.28000000000000003</v>
+      <c r="J149" s="11">
+        <v>1.3</v>
       </c>
       <c r="K149" s="11">
         <v>1.0900000000000001</v>
@@ -39684,8 +39740,8 @@
       <c r="I150" s="11">
         <v>0.99</v>
       </c>
-      <c r="J150" s="12">
-        <v>0.75</v>
+      <c r="J150" s="11">
+        <v>1.31</v>
       </c>
       <c r="K150" s="12">
         <v>0.77</v>
@@ -39723,7 +39779,7 @@
         <v>0.67</v>
       </c>
       <c r="J151" s="12">
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="K151" s="12">
         <v>0.72</v>
@@ -39760,8 +39816,8 @@
       <c r="I152" s="11">
         <v>0.99</v>
       </c>
-      <c r="J152" s="12">
-        <v>0.48</v>
+      <c r="J152" s="11">
+        <v>1.46</v>
       </c>
       <c r="K152" s="11">
         <v>0.95</v>
@@ -39799,7 +39855,7 @@
         <v>0.93</v>
       </c>
       <c r="J153" s="12">
-        <v>0.33</v>
+        <v>0.84</v>
       </c>
       <c r="K153" s="12">
         <v>0.57999999999999996</v>
@@ -39836,8 +39892,8 @@
       <c r="I154" s="11">
         <v>1.17</v>
       </c>
-      <c r="J154" s="12">
-        <v>0</v>
+      <c r="J154" s="11">
+        <v>0.96</v>
       </c>
       <c r="K154" s="11">
         <v>1.17</v>
@@ -39875,7 +39931,7 @@
         <v>0.71</v>
       </c>
       <c r="J155" s="12">
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="K155" s="11">
         <v>1.03</v>
@@ -39950,8 +40006,8 @@
       <c r="I157" s="11">
         <v>1.06</v>
       </c>
-      <c r="J157" s="12">
-        <v>0</v>
+      <c r="J157" s="11">
+        <v>0.92</v>
       </c>
       <c r="K157" s="11">
         <v>1.03</v>
@@ -39988,8 +40044,8 @@
       <c r="I158" s="11">
         <v>0.94</v>
       </c>
-      <c r="J158" s="12">
-        <v>0</v>
+      <c r="J158" s="11">
+        <v>0.96</v>
       </c>
       <c r="K158" s="11">
         <v>1.1000000000000001</v>
@@ -40027,10 +40083,10 @@
         <v>0.46</v>
       </c>
       <c r="J159" s="12">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="K159" s="11">
-        <v>1.08</v>
+        <v>1.02</v>
       </c>
       <c r="L159" s="11">
         <v>1.1499999999999999</v>
@@ -40064,8 +40120,8 @@
       <c r="I160" s="11">
         <v>1.04</v>
       </c>
-      <c r="J160" s="12">
-        <v>0</v>
+      <c r="J160" s="11">
+        <v>0.94</v>
       </c>
       <c r="K160" s="11">
         <v>1.04</v>
@@ -40103,7 +40159,7 @@
         <v>1.07</v>
       </c>
       <c r="J161" s="12">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="K161" s="11">
         <v>1.07</v>
@@ -40141,7 +40197,7 @@
         <v>0.67</v>
       </c>
       <c r="J162" s="12">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="K162" s="11">
         <v>1.08</v>
@@ -40179,7 +40235,7 @@
         <v>1.07</v>
       </c>
       <c r="J163" s="12">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="K163" s="11">
         <v>0.99</v>
@@ -40217,7 +40273,7 @@
         <v>1.01</v>
       </c>
       <c r="J164" s="12">
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="K164" s="11">
         <v>0.93</v>
@@ -40254,8 +40310,8 @@
       <c r="I165" s="11">
         <v>1.08</v>
       </c>
-      <c r="J165" s="12">
-        <v>0</v>
+      <c r="J165" s="11">
+        <v>0.97</v>
       </c>
       <c r="K165" s="11">
         <v>1.1100000000000001</v>
@@ -40292,8 +40348,8 @@
       <c r="I166" s="11">
         <v>1.1200000000000001</v>
       </c>
-      <c r="J166" s="12">
-        <v>0</v>
+      <c r="J166" s="11">
+        <v>0.95</v>
       </c>
       <c r="K166" s="11">
         <v>1.17</v>
@@ -40324,14 +40380,14 @@
       <c r="G167" s="11">
         <v>0.93</v>
       </c>
-      <c r="H167" s="12">
-        <v>0.13</v>
+      <c r="H167" s="11">
+        <v>1.1599999999999999</v>
       </c>
       <c r="I167" s="12">
         <v>0</v>
       </c>
-      <c r="J167" s="12">
-        <v>0</v>
+      <c r="J167" s="11">
+        <v>0.93</v>
       </c>
       <c r="K167" s="11">
         <v>0.99</v>
@@ -40369,7 +40425,7 @@
         <v>1.01</v>
       </c>
       <c r="J168" s="12">
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="K168" s="11">
         <v>1</v>
@@ -40407,7 +40463,7 @@
         <v>0.97</v>
       </c>
       <c r="J169" s="12">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="K169" s="11">
         <v>1.01</v>
@@ -40444,8 +40500,8 @@
       <c r="I170" s="12">
         <v>0.87</v>
       </c>
-      <c r="J170" s="12">
-        <v>0</v>
+      <c r="J170" s="11">
+        <v>0.95</v>
       </c>
       <c r="K170" s="11">
         <v>1.04</v>
@@ -40483,7 +40539,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J171" s="12">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="K171" s="11">
         <v>1.07</v>
@@ -40520,8 +40576,8 @@
       <c r="I172" s="11">
         <v>1.1100000000000001</v>
       </c>
-      <c r="J172" s="12">
-        <v>0</v>
+      <c r="J172" s="11">
+        <v>1</v>
       </c>
       <c r="K172" s="11">
         <v>1.04</v>
@@ -40559,7 +40615,7 @@
         <v>0.64</v>
       </c>
       <c r="J173" s="12">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K173" s="12">
         <v>0.48</v>
@@ -40597,7 +40653,7 @@
         <v>0.96</v>
       </c>
       <c r="J174" s="12">
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="K174" s="11">
         <v>0.99</v>
@@ -40635,7 +40691,7 @@
         <v>0.68</v>
       </c>
       <c r="J175" s="12">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="K175" s="12">
         <v>0</v>
@@ -40673,7 +40729,7 @@
         <v>0.11</v>
       </c>
       <c r="J176" s="12">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="K176" s="12">
         <v>0</v>
@@ -40711,7 +40767,7 @@
         <v>0.65</v>
       </c>
       <c r="J177" s="12">
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="K177" s="11">
         <v>1.02</v>
@@ -40787,7 +40843,7 @@
         <v>0.67</v>
       </c>
       <c r="J179" s="12">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="K179" s="12">
         <v>0.72</v>
@@ -40824,8 +40880,8 @@
       <c r="I180" s="11">
         <v>1.07</v>
       </c>
-      <c r="J180" s="12">
-        <v>0</v>
+      <c r="J180" s="11">
+        <v>1.02</v>
       </c>
       <c r="K180" s="12">
         <v>0.69</v>
@@ -40863,7 +40919,7 @@
         <v>1.01</v>
       </c>
       <c r="J181" s="12">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="K181" s="11">
         <v>1</v>
@@ -40901,7 +40957,7 @@
         <v>1.01</v>
       </c>
       <c r="J182" s="12">
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="K182" s="11">
         <v>1</v>
@@ -40939,7 +40995,7 @@
         <v>0.66</v>
       </c>
       <c r="J183" s="12">
-        <v>0.68</v>
+        <v>0.85</v>
       </c>
       <c r="K183" s="12">
         <v>0.67</v>
@@ -41014,8 +41070,8 @@
       <c r="I185" s="11">
         <v>0.95</v>
       </c>
-      <c r="J185" s="12">
-        <v>0.76</v>
+      <c r="J185" s="11">
+        <v>0.94</v>
       </c>
       <c r="K185" s="11">
         <v>0.93</v>
@@ -41091,7 +41147,7 @@
         <v>1.04</v>
       </c>
       <c r="J187" s="11">
-        <v>0.97</v>
+        <v>1.21</v>
       </c>
       <c r="K187" s="11">
         <v>1.03</v>
@@ -41128,8 +41184,8 @@
       <c r="I188" s="11">
         <v>0.92</v>
       </c>
-      <c r="J188" s="12">
-        <v>0.78</v>
+      <c r="J188" s="11">
+        <v>0.97</v>
       </c>
       <c r="K188" s="11">
         <v>1</v>
@@ -41167,7 +41223,7 @@
         <v>0</v>
       </c>
       <c r="J189" s="11">
-        <v>0.98</v>
+        <v>1.22</v>
       </c>
       <c r="K189" s="11">
         <v>0.99</v>
@@ -41205,7 +41261,7 @@
         <v>1.02</v>
       </c>
       <c r="J190" s="12">
-        <v>0.68</v>
+        <v>0.85</v>
       </c>
       <c r="K190" s="12">
         <v>0.55000000000000004</v>
@@ -41243,7 +41299,7 @@
         <v>0.99</v>
       </c>
       <c r="J191" s="12">
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="K191" s="12">
         <v>0.43</v>
@@ -41280,8 +41336,8 @@
       <c r="I192" s="11">
         <v>0.93</v>
       </c>
-      <c r="J192" s="12">
-        <v>0.75</v>
+      <c r="J192" s="11">
+        <v>0.94</v>
       </c>
       <c r="K192" s="11">
         <v>0.91</v>
@@ -41319,7 +41375,7 @@
         <v>0.44</v>
       </c>
       <c r="J193" s="12">
-        <v>0.34</v>
+        <v>0.43</v>
       </c>
       <c r="K193" s="12">
         <v>0.59</v>
@@ -41357,7 +41413,7 @@
         <v>0.97</v>
       </c>
       <c r="J194" s="12">
-        <v>0.63</v>
+        <v>0.79</v>
       </c>
       <c r="K194" s="12">
         <v>0.88</v>
@@ -41394,8 +41450,8 @@
       <c r="I195" s="11">
         <v>1.1200000000000001</v>
       </c>
-      <c r="J195" s="12">
-        <v>0.89</v>
+      <c r="J195" s="11">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K195" s="12">
         <v>0.23</v>
@@ -41433,7 +41489,7 @@
         <v>0.98</v>
       </c>
       <c r="J196" s="11">
-        <v>0.97</v>
+        <v>1.22</v>
       </c>
       <c r="K196" s="11">
         <v>1</v>
@@ -41470,8 +41526,8 @@
       <c r="I197" s="11">
         <v>0.96</v>
       </c>
-      <c r="J197" s="12">
-        <v>0.89</v>
+      <c r="J197" s="11">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K197" s="12">
         <v>0.71</v>
@@ -41508,8 +41564,8 @@
       <c r="I198" s="12">
         <v>0.84</v>
       </c>
-      <c r="J198" s="12">
-        <v>0.73</v>
+      <c r="J198" s="11">
+        <v>0.92</v>
       </c>
       <c r="K198" s="12">
         <v>0.61</v>
@@ -41546,8 +41602,8 @@
       <c r="I199" s="12">
         <v>0.88</v>
       </c>
-      <c r="J199" s="12">
-        <v>0.89</v>
+      <c r="J199" s="11">
+        <v>1.1100000000000001</v>
       </c>
       <c r="K199" s="12">
         <v>0.79</v>
@@ -41585,7 +41641,7 @@
         <v>0.86</v>
       </c>
       <c r="J200" s="12">
-        <v>0.66</v>
+        <v>0.82</v>
       </c>
       <c r="K200" s="12">
         <v>0.83</v>
@@ -41623,7 +41679,7 @@
         <v>0.6</v>
       </c>
       <c r="J201" s="11">
-        <v>0.97</v>
+        <v>1.21</v>
       </c>
       <c r="K201" s="11">
         <v>0.92</v>
@@ -41661,7 +41717,7 @@
         <v>0.69</v>
       </c>
       <c r="J202" s="12">
-        <v>0.56000000000000005</v>
+        <v>0.7</v>
       </c>
       <c r="K202" s="12">
         <v>0</v>
@@ -41699,7 +41755,7 @@
         <v>1.01</v>
       </c>
       <c r="J203" s="11">
-        <v>1.01</v>
+        <v>1.26</v>
       </c>
       <c r="K203" s="11">
         <v>1.05</v>
@@ -41737,7 +41793,7 @@
         <v>1.06</v>
       </c>
       <c r="J204" s="12">
-        <v>0.62</v>
+        <v>0.77</v>
       </c>
       <c r="K204" s="12">
         <v>0.42</v>
@@ -41774,8 +41830,8 @@
       <c r="I205" s="11">
         <v>0.98</v>
       </c>
-      <c r="J205" s="12">
-        <v>0.73</v>
+      <c r="J205" s="11">
+        <v>0.91</v>
       </c>
       <c r="K205" s="11">
         <v>0.9</v>
@@ -41812,8 +41868,8 @@
       <c r="I206" s="11">
         <v>1.02</v>
       </c>
-      <c r="J206" s="12">
-        <v>0.88</v>
+      <c r="J206" s="11">
+        <v>1.1000000000000001</v>
       </c>
       <c r="K206" s="11">
         <v>1</v>
@@ -41851,7 +41907,7 @@
         <v>0.81</v>
       </c>
       <c r="J207" s="11">
-        <v>0.91</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="K207" s="12">
         <v>0.72</v>
@@ -41889,7 +41945,7 @@
         <v>1.05</v>
       </c>
       <c r="J208" s="11">
-        <v>0.95</v>
+        <v>1.19</v>
       </c>
       <c r="K208" s="11">
         <v>0.98</v>
@@ -41926,8 +41982,8 @@
       <c r="I209" s="11">
         <v>1.01</v>
       </c>
-      <c r="J209" s="12">
-        <v>0.8</v>
+      <c r="J209" s="11">
+        <v>1</v>
       </c>
       <c r="K209" s="11">
         <v>1</v>
@@ -41965,7 +42021,7 @@
         <v>0.96</v>
       </c>
       <c r="J210" s="11">
-        <v>0.97</v>
+        <v>1.21</v>
       </c>
       <c r="K210" s="11">
         <v>0.92</v>
@@ -42003,7 +42059,7 @@
         <v>0.95</v>
       </c>
       <c r="J211" s="11">
-        <v>1.02</v>
+        <v>1.28</v>
       </c>
       <c r="K211" s="12">
         <v>0.88</v>
@@ -42041,7 +42097,7 @@
         <v>1</v>
       </c>
       <c r="J212" s="12">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="K212" s="11">
         <v>1</v>
@@ -42079,7 +42135,7 @@
         <v>0.68</v>
       </c>
       <c r="J213" s="12">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="K213" s="11">
         <v>1</v>
@@ -42117,7 +42173,7 @@
         <v>1</v>
       </c>
       <c r="J214" s="12">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="K214" s="11">
         <v>1</v>
@@ -42155,7 +42211,7 @@
         <v>1</v>
       </c>
       <c r="J215" s="12">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="K215" s="11">
         <v>1</v>
@@ -42193,13 +42249,13 @@
         <v>0.85</v>
       </c>
       <c r="J216" s="12">
-        <v>-0.19</v>
+        <v>0.82</v>
       </c>
       <c r="K216" s="12">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="L216" s="12">
-        <v>0.65</v>
+        <v>0.79</v>
+      </c>
+      <c r="L216" s="11">
+        <v>0.92</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -42230,8 +42286,8 @@
       <c r="I217" s="11">
         <v>0.98</v>
       </c>
-      <c r="J217" s="12">
-        <v>0.15</v>
+      <c r="J217" s="11">
+        <v>1.27</v>
       </c>
       <c r="K217" s="11">
         <v>1.04</v>
@@ -42269,13 +42325,13 @@
         <v>0</v>
       </c>
       <c r="J218" s="12">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="K218" s="11">
         <v>1.24</v>
       </c>
-      <c r="L218" s="12">
-        <v>0.15</v>
+      <c r="L218" s="11">
+        <v>0.92</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -42307,13 +42363,13 @@
         <v>0.96</v>
       </c>
       <c r="J219" s="12">
-        <v>0.33</v>
-      </c>
-      <c r="K219" s="12">
-        <v>0.16</v>
-      </c>
-      <c r="L219" s="12">
-        <v>0.18</v>
+        <v>0.84</v>
+      </c>
+      <c r="K219" s="11">
+        <v>1.01</v>
+      </c>
+      <c r="L219" s="11">
+        <v>1.01</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
@@ -42345,10 +42401,10 @@
         <v>1.01</v>
       </c>
       <c r="J220" s="12">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="K220" s="12">
-        <v>0.68</v>
+        <v>0.88</v>
       </c>
       <c r="L220" s="12">
         <v>0.79</v>
@@ -42382,11 +42438,11 @@
       <c r="I221" s="11">
         <v>1</v>
       </c>
-      <c r="J221" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="K221" s="12">
-        <v>0.12</v>
+      <c r="J221" s="11">
+        <v>1.37</v>
+      </c>
+      <c r="K221" s="11">
+        <v>0.96</v>
       </c>
       <c r="L221" s="12">
         <v>0.64</v>
@@ -42420,11 +42476,11 @@
       <c r="I222" s="11">
         <v>1.02</v>
       </c>
-      <c r="J222" s="12">
-        <v>0.49</v>
+      <c r="J222" s="11">
+        <v>1.33</v>
       </c>
       <c r="K222" s="11">
-        <v>1.08</v>
+        <v>1.26</v>
       </c>
       <c r="L222" s="11">
         <v>1.23</v>
@@ -42497,10 +42553,10 @@
         <v>1.01</v>
       </c>
       <c r="J224" s="12">
-        <v>-0.26</v>
-      </c>
-      <c r="K224" s="12">
-        <v>0.46</v>
+        <v>0.59</v>
+      </c>
+      <c r="K224" s="11">
+        <v>1.06</v>
       </c>
       <c r="L224" s="11">
         <v>0.95</v>
@@ -42535,13 +42591,13 @@
         <v>1.02</v>
       </c>
       <c r="J225" s="12">
-        <v>-0.49</v>
-      </c>
-      <c r="K225" s="12">
-        <v>0.23</v>
-      </c>
-      <c r="L225" s="12">
-        <v>0.18</v>
+        <v>0.9</v>
+      </c>
+      <c r="K225" s="11">
+        <v>1.05</v>
+      </c>
+      <c r="L225" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -42572,8 +42628,8 @@
       <c r="I226" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J226" s="12">
-        <v>0.32</v>
+      <c r="J226" s="11">
+        <v>1.23</v>
       </c>
       <c r="K226" s="11">
         <v>0.95</v>
@@ -42610,11 +42666,11 @@
       <c r="I227" s="11">
         <v>1.02</v>
       </c>
-      <c r="J227" s="12">
-        <v>-0.33</v>
+      <c r="J227" s="11">
+        <v>1.22</v>
       </c>
       <c r="K227" s="11">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="L227" s="12">
         <v>0.89</v>
@@ -42649,13 +42705,13 @@
         <v>0.91</v>
       </c>
       <c r="J228" s="12">
-        <v>-0.44</v>
+        <v>0.89</v>
       </c>
       <c r="K228" s="11">
-        <v>1.08</v>
-      </c>
-      <c r="L228" s="12">
-        <v>0.2</v>
+        <v>1.35</v>
+      </c>
+      <c r="L228" s="11">
+        <v>1.02</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -42686,8 +42742,8 @@
       <c r="I229" s="11">
         <v>1.02</v>
       </c>
-      <c r="J229" s="12">
-        <v>0.4</v>
+      <c r="J229" s="11">
+        <v>1.04</v>
       </c>
       <c r="K229" s="12">
         <v>0.85</v>
@@ -64496,6 +64552,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="3cef09ca-690e-48ca-8db1-bbccdf684368" xsi:nil="true"/>
@@ -64506,7 +64571,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C055B46FD48B3346B10CEACF6165CA2E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ce32beb785b16a844e5ac9984a39cddd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2ba1b9e1-d32c-453a-80ca-da429ca95d13" xmlns:ns3="3cef09ca-690e-48ca-8db1-bbccdf684368" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="929a4414321bae1528947cb08dec1f5d" ns2:_="" ns3:_="">
     <xsd:import namespace="2ba1b9e1-d32c-453a-80ca-da429ca95d13"/>
@@ -64761,16 +64826,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EF37548-399B-4B64-AB6C-62FF5630FEED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA11991-CB2B-42C8-9D1A-27999BA19AA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3cef09ca-690e-48ca-8db1-bbccdf684368"/>
@@ -64787,7 +64851,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835DC02C-D0D2-4615-ADA0-1E9180E8CC6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -64804,12 +64868,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EF37548-399B-4B64-AB6C-62FF5630FEED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>